<commit_message>
recovered glider 383. added recovered ingest sheet and updated cal info with recovered date.
</commit_message>
<xml_diff>
--- a/CE05MOAS-GL383/Omaha_Cal_Info_CE05MOAS-GL383_00002.xlsx
+++ b/CE05MOAS-GL383/Omaha_Cal_Info_CE05MOAS-GL383_00002.xlsx
@@ -35,7 +35,7 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$A$1:$J$77</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$319</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -744,7 +744,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,13 +807,13 @@
         <v>2</v>
       </c>
       <c r="D2" s="5">
-        <v>42025</v>
+        <v>42229</v>
       </c>
       <c r="E2" s="6">
         <v>0.88124999999999998</v>
       </c>
       <c r="F2" s="5">
-        <v>42229</v>
+        <v>42333</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>32</v>

</xml_diff>